<commit_message>
- Updated BOM (all components in stock on LCSC on 2/6/2020) - PickAndPlace in xlsx format
</commit_message>
<xml_diff>
--- a/bin/PCB/BOM_TSDZ2-ESP32.xlsx
+++ b/bin/PCB/BOM_TSDZ2-ESP32.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-ESP32-PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5A7CFE-51AD-4686-9797-B75653B4CD92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A005FD-391D-4E50-AAF4-FD3BEFBD2FE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="216" yWindow="792" windowWidth="22128" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3792" yWindow="1176" windowWidth="19248" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_TSDZ2-ESP32-v3" sheetId="1" r:id="rId1"/>
@@ -88,15 +88,9 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>RC-02W3093FT</t>
-  </si>
-  <si>
     <t>Guangdong Fenghua Advanced Tech</t>
   </si>
   <si>
-    <t>C321438</t>
-  </si>
-  <si>
     <t>CHIP RES. 309K Ohm 1%  1/16W 0402</t>
   </si>
   <si>
@@ -518,6 +512,12 @@
   </si>
   <si>
     <t>CHIP RES. 100K Ohm 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>WR04X3093FTL</t>
+  </si>
+  <si>
+    <t>C334683</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1361,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,19 +1467,19 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1487,31 +1487,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
         <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1519,31 +1519,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1551,31 +1551,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
         <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1583,31 +1583,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
         <v>48</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" t="s">
-        <v>50</v>
       </c>
       <c r="K7" t="s">
         <v>18</v>
@@ -1618,10 +1618,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -1630,19 +1630,19 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" t="s">
         <v>53</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1650,10 +1650,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -1662,19 +1662,19 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
         <v>58</v>
       </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1682,31 +1682,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
         <v>65</v>
-      </c>
-      <c r="H10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J10" t="s">
-        <v>67</v>
       </c>
       <c r="K10" t="s">
         <v>18</v>
@@ -1717,31 +1717,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
         <v>70</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>71</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1749,31 +1749,31 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
         <v>74</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
         <v>77</v>
       </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>78</v>
-      </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1781,31 +1781,31 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
         <v>83</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>84</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1813,31 +1813,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
         <v>87</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" t="s">
         <v>89</v>
-      </c>
-      <c r="H14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1845,31 +1845,31 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
         <v>92</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" t="s">
-        <v>94</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1877,31 +1877,31 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
         <v>99</v>
       </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
         <v>100</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>101</v>
-      </c>
-      <c r="J16" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1909,31 +1909,31 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
         <v>103</v>
       </c>
-      <c r="G17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" t="s">
-        <v>105</v>
-      </c>
       <c r="J17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1941,31 +1941,31 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
         <v>107</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" t="s">
-        <v>109</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
         <v>110</v>
       </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
         <v>111</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" t="s">
-        <v>112</v>
-      </c>
-      <c r="J18" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1973,31 +1973,31 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" t="s">
         <v>114</v>
-      </c>
-      <c r="C19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" t="s">
-        <v>116</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K19" t="s">
         <v>18</v>
@@ -2008,31 +2008,31 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D20" t="s">
         <v>119</v>
-      </c>
-      <c r="C20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20" t="s">
-        <v>121</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2040,31 +2040,31 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
         <v>126</v>
       </c>
-      <c r="G21" t="s">
+      <c r="J21" t="s">
         <v>127</v>
-      </c>
-      <c r="H21" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" t="s">
-        <v>128</v>
-      </c>
-      <c r="J21" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2072,31 +2072,31 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
         <v>130</v>
-      </c>
-      <c r="C22" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" t="s">
-        <v>132</v>
       </c>
       <c r="E22">
         <v>7</v>
       </c>
       <c r="F22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
         <v>133</v>
       </c>
-      <c r="G22" t="s">
+      <c r="J22" t="s">
         <v>134</v>
-      </c>
-      <c r="H22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" t="s">
-        <v>135</v>
-      </c>
-      <c r="J22" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2107,7 +2107,7 @@
         <v>360</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
@@ -2116,19 +2116,19 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
         <v>138</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
         <v>139</v>
-      </c>
-      <c r="H23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -2136,34 +2136,34 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" t="s">
         <v>142</v>
-      </c>
-      <c r="C24" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" t="s">
-        <v>144</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
       </c>
       <c r="I24" t="s">
+        <v>143</v>
+      </c>
+      <c r="J24" t="s">
+        <v>144</v>
+      </c>
+      <c r="K24" t="s">
         <v>145</v>
-      </c>
-      <c r="J24" t="s">
-        <v>146</v>
-      </c>
-      <c r="K24" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -2171,31 +2171,31 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" t="s">
         <v>148</v>
-      </c>
-      <c r="C25" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" t="s">
-        <v>150</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" t="s">
         <v>151</v>
       </c>
-      <c r="G25" t="s">
+      <c r="J25" t="s">
         <v>152</v>
-      </c>
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" t="s">
-        <v>153</v>
-      </c>
-      <c r="J25" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -2203,31 +2203,31 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" t="s">
         <v>155</v>
-      </c>
-      <c r="C26" t="s">
-        <v>156</v>
-      </c>
-      <c r="D26" t="s">
-        <v>157</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" t="s">
+        <v>157</v>
+      </c>
+      <c r="J26" t="s">
         <v>158</v>
-      </c>
-      <c r="H26" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" t="s">
-        <v>159</v>
-      </c>
-      <c r="J26" t="s">
-        <v>160</v>
       </c>
       <c r="K26" t="s">
         <v>18</v>
@@ -2238,10 +2238,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -2250,19 +2250,19 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>162</v>
+      </c>
+      <c r="J27" t="s">
         <v>163</v>
-      </c>
-      <c r="G27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" t="s">
-        <v>164</v>
-      </c>
-      <c r="J27" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>